<commit_message>
Added new ammo types, added a shotgun chart, and updated chest hp to be 85 instead of 80, and updated limits for the chart
</commit_message>
<xml_diff>
--- a/pistol.xlsx
+++ b/pistol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack-\Documents\Code\Funny Ammo Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1C65788-C730-49F3-90AF-E0972BAB77F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A598AE20-AD62-41B7-B0FC-085FC6F3F7CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6C20383B-5001-4866-817D-564901780D4C}"/>
+    <workbookView xWindow="6450" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{6C20383B-5001-4866-817D-564901780D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>7.62x25mm</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>SP8 gzh</t>
+  </si>
+  <si>
+    <t>7n31</t>
+  </si>
+  <si>
+    <t>Quakemaker</t>
   </si>
 </sst>
 </file>
@@ -600,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D568D7A5-5F59-4170-8D5E-267D968BE42A}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,239 +1015,267 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C29" s="7">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D29" s="7">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C30" s="7">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="D30" s="7">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="7">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D31" s="7">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="7">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D32" s="7">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="7">
+        <v>80</v>
+      </c>
+      <c r="D33" s="7">
         <v>15</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="7">
-        <v>72</v>
-      </c>
-      <c r="D33" s="7">
-        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C34" s="7">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="D34" s="7">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C35" s="7">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D35" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C36" s="7">
-        <v>35</v>
+        <v>127</v>
       </c>
       <c r="D36" s="7">
-        <v>53</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C37" s="7">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D37" s="7">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="7">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D38" s="7">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C39" s="7">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D39" s="7">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C40" s="7">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="D40" s="7">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C41" s="7">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D41" s="7">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C42" s="7">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="D42" s="7">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C43" s="7">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="D43" s="7">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C44" s="7">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D44" s="7">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="7">
+        <v>49</v>
+      </c>
+      <c r="D45" s="7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="7">
+        <v>62</v>
+      </c>
+      <c r="D46" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="7">
         <v>74</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D47" s="7">
         <v>10</v>
       </c>
     </row>

</xml_diff>